<commit_message>
Changed wing_AR from being a parameter into a design variable
</commit_message>
<xml_diff>
--- a/sheets/estimate_energy.xlsx
+++ b/sheets/estimate_energy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF242EC1-E257-0747-8E7A-AD68B209C3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB4D137-246F-E848-ACD7-42E5935E30AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="15080" windowHeight="18900" xr2:uid="{843CD013-835A-1741-B375-CD508AE79BD2}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="15080" windowHeight="18900" activeTab="1" xr2:uid="{843CD013-835A-1741-B375-CD508AE79BD2}"/>
   </bookViews>
   <sheets>
     <sheet name="multirotor" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="93">
   <si>
     <t>!!! Press F9 to recalculate !!!</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>hover_FM</t>
-  </si>
-  <si>
-    <t>Wing parameters</t>
   </si>
   <si>
     <t>Cd0</t>
@@ -420,15 +417,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,7 +762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB60D980-77E2-5F49-A087-DF4F0ECC2A24}">
   <dimension ref="B1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -794,90 +791,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="2:25" x14ac:dyDescent="0.2">
       <c r="P2" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="F3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="J3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="P3" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B3" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="F3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="J3" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="Y3" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G4">
         <f xml:space="preserve"> 1/$C$7 * SQRT( ($C$15*$C$26)^3 / (2 * $C$25 * PI() * $C$16^2* $C$5) )</f>
         <v>270203.45112999814</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K4">
         <f xml:space="preserve"> 0.5 * $C$25 * $C$17^2</f>
         <v>551.25</v>
       </c>
       <c r="L4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P4" s="7">
         <v>0</v>
@@ -919,30 +916,30 @@
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1">
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5">
         <f>$C$15*$C$26/$C$5</f>
         <v>2102.1428571428573</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K5">
         <f xml:space="preserve"> 0.0327 * ($C$15*2.20462)^0.8903 * 0.3048^2</f>
         <v>4.1297309384395309</v>
       </c>
       <c r="L5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P5" s="7">
         <v>1</v>
@@ -992,7 +989,7 @@
         <v>0.13</v>
       </c>
       <c r="J6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K6">
         <f xml:space="preserve"> K5 / ($C$5 * PI() * $C$16^2)</f>
@@ -1045,20 +1042,20 @@
       <c r="C7" s="1">
         <v>0.75</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
+      <c r="F7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
       <c r="J7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K7">
         <f xml:space="preserve"> K4 * K5</f>
         <v>2276.5141798147915</v>
       </c>
       <c r="L7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P7" s="7">
         <v>3</v>
@@ -1102,24 +1099,24 @@
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.2">
       <c r="F8" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G8">
         <f xml:space="preserve"> K22 + K18 * (K27 * K24 + $C$17 * SIN(K17))</f>
         <v>27867.298973721139</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K8">
         <f>K7</f>
         <v>2276.5141798147915</v>
       </c>
       <c r="L8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P8" s="7">
         <v>4</v>
@@ -1162,20 +1159,20 @@
       </c>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
+      <c r="B9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
       <c r="F9" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9">
         <f>$C$5 * G8</f>
         <v>195071.09281604798</v>
       </c>
       <c r="H9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P9" s="7">
         <v>5</v>
@@ -1219,13 +1216,13 @@
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
         <v>280</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P10" s="7">
         <v>6</v>
@@ -1269,18 +1266,18 @@
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1">
         <v>0.85</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="J11" s="9" t="s">
-        <v>91</v>
+      <c r="F11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="J11" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
@@ -1326,30 +1323,30 @@
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1">
         <v>0.8</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G12">
         <f xml:space="preserve"> (G4*$C$22 + G9*G13)/3600</f>
         <v>27044.632520520616</v>
       </c>
       <c r="H12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K12">
         <f xml:space="preserve"> SQRT( ($C$15*$C$26)^2 + K8^2)</f>
         <v>14890.055131224257</v>
       </c>
       <c r="L12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P12" s="7">
         <v>8</v>
@@ -1393,17 +1390,17 @@
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.2">
       <c r="F13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13">
         <f xml:space="preserve"> $C$21 / $C$17</f>
         <v>166.66666666666666</v>
       </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K13">
         <f>$C$15*$C$26/K12</f>
@@ -1450,11 +1447,11 @@
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B14" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="B14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
       <c r="P14" s="7">
         <v>10</v>
       </c>
@@ -1497,13 +1494,13 @@
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="2">
         <v>1500</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P15" s="7">
         <v>11</v>
@@ -1547,16 +1544,16 @@
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1">
         <v>1.2</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>50</v>
+        <v>15</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
@@ -1602,23 +1599,23 @@
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1">
         <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K17">
         <f xml:space="preserve"> ACOS(K13)</f>
         <v>0.15349020639723854</v>
       </c>
       <c r="L17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P17" s="7">
         <v>13</v>
@@ -1662,20 +1659,20 @@
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="1">
         <v>0.3</v>
       </c>
       <c r="J18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K18">
         <f xml:space="preserve"> K12 / $C$5</f>
         <v>2127.1507330320369</v>
       </c>
       <c r="L18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P18" s="7">
         <v>14</v>
@@ -1719,14 +1716,14 @@
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.2">
       <c r="J19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K19">
         <f xml:space="preserve"> $C$17 * COS(K17) / ($C$18 * $C$16)</f>
         <v>82.353623891463599</v>
       </c>
       <c r="L19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P19" s="7">
         <v>15</v>
@@ -1769,13 +1766,13 @@
       </c>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B20" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
+      <c r="B20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
       <c r="J20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K20">
         <f xml:space="preserve"> K18 / ($C$25 * PI() * $C$16^2 * K19^2 * $C$16^2)</f>
@@ -1823,16 +1820,16 @@
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="1">
         <v>5000</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K21" s="1">
         <v>1.2E-2</v>
@@ -1879,23 +1876,23 @@
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="1">
         <v>240</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K22">
         <f xml:space="preserve"> ($C$6 * K21 / 8) * (1 + 4.65 *$C$18^ 2) * ( PI() * $C$25 * K19^3 *$C$16^ 5)</f>
         <v>1479.463608760032</v>
       </c>
       <c r="L22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P22" s="7">
         <v>18</v>
@@ -1939,7 +1936,7 @@
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.2">
       <c r="J23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K23" s="4">
         <f>U34</f>
@@ -1986,20 +1983,20 @@
       </c>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B24" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
+      <c r="B24" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
       <c r="J24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K24">
         <f xml:space="preserve"> K19 * $C$16 * K23 - $C$17 * SIN(K17)</f>
         <v>6.0905011857570672</v>
       </c>
       <c r="L24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P24" s="7">
         <v>20</v>
@@ -2043,16 +2040,16 @@
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1">
         <v>1.2250000000000001</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K25">
         <f xml:space="preserve"> 1/$C$7 - K22 * SQRT( (2*$C$25*PI()*$C$16^2) / K18^3 )</f>
@@ -2100,16 +2097,16 @@
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="1">
         <v>9.81</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K26" s="1">
         <v>1.1499999999999999</v>
@@ -2156,7 +2153,7 @@
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.2">
       <c r="J27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K27">
         <f xml:space="preserve"> 1/$C$29 * LN( EXP($C$29 * K25) + EXP($C$29 * K26) )</f>
@@ -2203,11 +2200,11 @@
       </c>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B28" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
+      <c r="B28" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
       <c r="P28" s="7">
         <v>24</v>
       </c>
@@ -2250,7 +2247,7 @@
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="1">
         <v>30</v>
@@ -2522,10 +2519,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C46306-B19A-E840-A2A2-9C88BDE95F01}">
-  <dimension ref="B1:Y37"/>
+  <dimension ref="B1:Y35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2553,90 +2550,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="2:25" x14ac:dyDescent="0.2">
       <c r="P2" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="F3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="J3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="P3" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B3" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="F3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="J3" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="Y3" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4">
+        <f xml:space="preserve"> 1/$C$9 * SQRT( ($C$17*$C$31)^3 / (2 * $C$30 * PI() * $C$18^2* $C$5) )</f>
+        <v>350223.7005176876</v>
+      </c>
+      <c r="H4" t="s">
         <v>34</v>
       </c>
-      <c r="G4">
-        <f xml:space="preserve"> 1/$C$9 * SQRT( ($C$20*$C$33)^3 / (2 * $C$32 * PI() * $C$21^2* $C$5) )</f>
-        <v>291853.08376473968</v>
-      </c>
-      <c r="H4" t="s">
-        <v>35</v>
-      </c>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K4">
-        <f xml:space="preserve"> $C$20 * $C$33</f>
+        <f xml:space="preserve"> $C$17 * $C$31</f>
         <v>14715</v>
       </c>
       <c r="L4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P4" s="7">
         <v>0</v>
@@ -2646,14 +2643,14 @@
       </c>
       <c r="R4" s="7">
         <f t="shared" ref="R4:R34" si="0" xml:space="preserve"> $K$19 * TAN($K$16) + $K$20 / (2 * SQRT($K$19^2 + Q4^2)) - Q4</f>
-        <v>0.58425088338188247</v>
+        <v>1.5020486687632517</v>
       </c>
       <c r="S4" s="8">
         <v>1</v>
       </c>
       <c r="T4" s="7">
         <f t="shared" ref="T4:T34" si="1" xml:space="preserve"> $K$19 * TAN($K$16) + $K$20 / (2 * SQRT($K$19^2 + S4^2)) - S4</f>
-        <v>-0.6754927486334632</v>
+        <v>-0.65004050461200347</v>
       </c>
       <c r="U4" s="7">
         <f xml:space="preserve"> (Q4 + S4)/2</f>
@@ -2661,15 +2658,15 @@
       </c>
       <c r="V4" s="7">
         <f t="shared" ref="V4:V34" si="2" xml:space="preserve"> $K$19 * TAN($K$16) + $K$20 / (2 * SQRT($K$19^2 + U4^2)) - U4</f>
-        <v>-0.16810118167500365</v>
+        <v>-0.1172553148422063</v>
       </c>
       <c r="W4" s="7">
         <f>R4*V4</f>
-        <v>-9.8213263891159197E-2</v>
+        <v>-0.17612318956415193</v>
       </c>
       <c r="X4" s="7">
         <f>T4*V4</f>
-        <v>0.11355112925818138</v>
+        <v>7.6220704028467132E-2</v>
       </c>
       <c r="Y4" s="7">
         <f>S4-Q4</f>
@@ -2678,30 +2675,30 @@
     </row>
     <row r="5" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1">
         <v>6</v>
       </c>
       <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5">
+        <f>$C$17*$C$31/$C$5</f>
+        <v>2452.5</v>
+      </c>
+      <c r="H5" t="s">
         <v>36</v>
       </c>
-      <c r="G5">
-        <f>$C$20*$C$33/$C$5</f>
-        <v>2452.5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>37</v>
-      </c>
       <c r="J5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5">
+        <f xml:space="preserve"> 0.5 * $C$30 * $C$20^2</f>
+        <v>551.25</v>
+      </c>
+      <c r="L5" t="s">
         <v>47</v>
-      </c>
-      <c r="K5">
-        <f xml:space="preserve"> 0.5 * $C$32 * $C$23^2</f>
-        <v>1852.8125000000002</v>
-      </c>
-      <c r="L5" t="s">
-        <v>48</v>
       </c>
       <c r="P5" s="7">
         <v>1</v>
@@ -2712,7 +2709,7 @@
       </c>
       <c r="R5" s="7">
         <f t="shared" si="0"/>
-        <v>0.58425088338188247</v>
+        <v>1.5020486687632517</v>
       </c>
       <c r="S5" s="7">
         <f>IF(X4&gt;0, U4, S4)</f>
@@ -2720,7 +2717,7 @@
       </c>
       <c r="T5" s="7">
         <f t="shared" si="1"/>
-        <v>-0.16810118167500365</v>
+        <v>-0.1172553148422063</v>
       </c>
       <c r="U5" s="7">
         <f t="shared" ref="U5:U34" si="3" xml:space="preserve"> (Q5 + S5)/2</f>
@@ -2728,15 +2725,15 @@
       </c>
       <c r="V5" s="7">
         <f t="shared" si="2"/>
-        <v>9.6563677734210207E-2</v>
+        <v>0.19779045980618776</v>
       </c>
       <c r="W5" s="7">
         <f t="shared" ref="W5:W34" si="4">R5*V5</f>
-        <v>5.6417414018815726E-2</v>
+        <v>0.29709089684595574</v>
       </c>
       <c r="X5" s="7">
         <f t="shared" ref="X5:X34" si="5">T5*V5</f>
-        <v>-1.6232468334004976E-2</v>
+        <v>-2.3191982637359297E-2</v>
       </c>
       <c r="Y5" s="7">
         <f t="shared" ref="Y5:Y34" si="6">S5-Q5</f>
@@ -2745,20 +2742,20 @@
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K6">
-        <f xml:space="preserve"> 1.6 * ($C$20*2.20462/1000)^(2/3) * 0.3048^2</f>
+        <f xml:space="preserve"> 1.6 * ($C$17*2.20462/1000)^(2/3) * 0.3048^2</f>
         <v>0.32993868766973189</v>
       </c>
       <c r="L6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P6" s="7">
         <v>2</v>
@@ -2769,7 +2766,7 @@
       </c>
       <c r="R6" s="7">
         <f t="shared" si="0"/>
-        <v>9.6563677734210207E-2</v>
+        <v>0.19779045980618776</v>
       </c>
       <c r="S6" s="7">
         <f t="shared" ref="S6:S34" si="8">IF(X5&gt;0, U5, S5)</f>
@@ -2777,7 +2774,7 @@
       </c>
       <c r="T6" s="7">
         <f t="shared" si="1"/>
-        <v>-0.16810118167500365</v>
+        <v>-0.1172553148422063</v>
       </c>
       <c r="U6" s="7">
         <f t="shared" si="3"/>
@@ -2785,15 +2782,15 @@
       </c>
       <c r="V6" s="7">
         <f t="shared" si="2"/>
-        <v>-3.8191293625573275E-2</v>
+        <v>2.9522423539072362E-2</v>
       </c>
       <c r="W6" s="7">
         <f t="shared" si="4"/>
-        <v>-3.6878917699124541E-3</v>
+        <v>5.8392537263861431E-3</v>
       </c>
       <c r="X6" s="7">
         <f t="shared" si="5"/>
-        <v>6.4200015881559023E-3</v>
+        <v>-3.4616610669788925E-3</v>
       </c>
       <c r="Y6" s="7">
         <f t="shared" si="6"/>
@@ -2807,52 +2804,52 @@
       <c r="C7" s="1">
         <v>0.13</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
+      <c r="F7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
       <c r="J7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K7">
-        <f xml:space="preserve"> K6 / $C$24</f>
-        <v>5.1552919948395608E-2</v>
+        <f xml:space="preserve"> K6 / $C$21</f>
+        <v>4.1242335958716486E-2</v>
       </c>
       <c r="P7" s="7">
         <v>3</v>
       </c>
       <c r="Q7" s="7">
         <f t="shared" si="7"/>
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="R7" s="7">
         <f t="shared" si="0"/>
-        <v>9.6563677734210207E-2</v>
+        <v>2.9522423539072362E-2</v>
       </c>
       <c r="S7" s="7">
         <f t="shared" si="8"/>
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="T7" s="7">
         <f t="shared" si="1"/>
-        <v>-3.8191293625573275E-2</v>
+        <v>-0.1172553148422063</v>
       </c>
       <c r="U7" s="7">
         <f t="shared" si="3"/>
-        <v>0.3125</v>
+        <v>0.4375</v>
       </c>
       <c r="V7" s="7">
         <f t="shared" si="2"/>
-        <v>2.8222450418169509E-2</v>
+        <v>-4.5412524688992817E-2</v>
       </c>
       <c r="W7" s="7">
         <f t="shared" si="4"/>
-        <v>2.7252636070498465E-3</v>
+        <v>-1.3406877878470262E-3</v>
       </c>
       <c r="X7" s="7">
         <f t="shared" si="5"/>
-        <v>-1.0778518907534949E-3</v>
+        <v>5.3248598801873201E-3</v>
       </c>
       <c r="Y7" s="7">
         <f t="shared" si="6"/>
@@ -2867,59 +2864,59 @@
         <v>0.13</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G8">
-        <f xml:space="preserve"> K22 + K17 * (K27 * K24 + $C$23 * SIN(K16))</f>
-        <v>84922.171492537891</v>
+        <f xml:space="preserve"> K22 + K17 * (K27 * K24 + $C$20 * SIN(K16))</f>
+        <v>90717.429803285791</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K8">
-        <f xml:space="preserve"> K5 * $C$24 * K7</f>
-        <v>611.3145247480752</v>
+        <f xml:space="preserve"> K5 * $C$21 * K7</f>
+        <v>181.87870157793969</v>
       </c>
       <c r="L8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P8" s="7">
         <v>4</v>
       </c>
       <c r="Q8" s="7">
         <f t="shared" si="7"/>
-        <v>0.3125</v>
+        <v>0.375</v>
       </c>
       <c r="R8" s="7">
         <f t="shared" si="0"/>
-        <v>2.8222450418169509E-2</v>
+        <v>2.9522423539072362E-2</v>
       </c>
       <c r="S8" s="7">
         <f t="shared" si="8"/>
-        <v>0.375</v>
+        <v>0.4375</v>
       </c>
       <c r="T8" s="7">
         <f t="shared" si="1"/>
-        <v>-3.8191293625573275E-2</v>
+        <v>-4.5412524688992817E-2</v>
       </c>
       <c r="U8" s="7">
         <f t="shared" si="3"/>
-        <v>0.34375</v>
+        <v>0.40625</v>
       </c>
       <c r="V8" s="7">
         <f t="shared" si="2"/>
-        <v>-5.1605827437828378E-3</v>
+        <v>-8.4199746806953302E-3</v>
       </c>
       <c r="W8" s="7">
         <f t="shared" si="4"/>
-        <v>-1.456442906152723E-4</v>
+        <v>-2.4857805871175313E-4</v>
       </c>
       <c r="X8" s="7">
         <f t="shared" si="5"/>
-        <v>1.9708933084687692E-4</v>
+        <v>3.8237230806777107E-4</v>
       </c>
       <c r="Y8" s="7">
         <f t="shared" si="6"/>
@@ -2934,20 +2931,20 @@
         <v>0.75</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9">
         <f xml:space="preserve"> $C$6 * G8</f>
-        <v>84922.171492537891</v>
+        <v>90717.429803285791</v>
       </c>
       <c r="H9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K9">
-        <f xml:space="preserve"> 1.78 * (1 - 0.045 * $C$12^0.68) - 0.64</f>
+        <f xml:space="preserve"> 1.78 * (1 - 0.045 * $C$22^0.68) - 0.64</f>
         <v>0.75661729604956662</v>
       </c>
       <c r="P9" s="7">
@@ -2955,35 +2952,35 @@
       </c>
       <c r="Q9" s="7">
         <f t="shared" si="7"/>
-        <v>0.3125</v>
+        <v>0.375</v>
       </c>
       <c r="R9" s="7">
         <f t="shared" si="0"/>
-        <v>2.8222450418169509E-2</v>
+        <v>2.9522423539072362E-2</v>
       </c>
       <c r="S9" s="7">
         <f t="shared" si="8"/>
-        <v>0.34375</v>
+        <v>0.40625</v>
       </c>
       <c r="T9" s="7">
         <f t="shared" si="1"/>
-        <v>-5.1605827437828378E-3</v>
+        <v>-8.4199746806953302E-3</v>
       </c>
       <c r="U9" s="7">
         <f t="shared" si="3"/>
-        <v>0.328125</v>
+        <v>0.390625</v>
       </c>
       <c r="V9" s="7">
         <f t="shared" si="2"/>
-        <v>1.1480688847282594E-2</v>
+        <v>1.0418385137178243E-2</v>
       </c>
       <c r="W9" s="7">
         <f t="shared" si="4"/>
-        <v>3.2401317175886468E-4</v>
+        <v>3.0757597861295259E-4</v>
       </c>
       <c r="X9" s="7">
         <f t="shared" si="5"/>
-        <v>-5.9247044752026633E-5</v>
+        <v>-8.7722539068773355E-5</v>
       </c>
       <c r="Y9" s="7">
         <f t="shared" si="6"/>
@@ -2992,46 +2989,46 @@
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.2">
       <c r="J10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K10">
-        <f xml:space="preserve"> K4 / (K5 * $C$24)</f>
-        <v>1.2409343902850394</v>
+        <f xml:space="preserve"> K4 / (K5 * $C$21)</f>
+        <v>3.3367346938775508</v>
       </c>
       <c r="P10" s="7">
         <v>6</v>
       </c>
       <c r="Q10" s="7">
         <f t="shared" si="7"/>
-        <v>0.328125</v>
+        <v>0.390625</v>
       </c>
       <c r="R10" s="7">
         <f t="shared" si="0"/>
-        <v>1.1480688847282594E-2</v>
+        <v>1.0418385137178243E-2</v>
       </c>
       <c r="S10" s="7">
         <f t="shared" si="8"/>
-        <v>0.34375</v>
+        <v>0.40625</v>
       </c>
       <c r="T10" s="7">
         <f t="shared" si="1"/>
-        <v>-5.1605827437828378E-3</v>
+        <v>-8.4199746806953302E-3</v>
       </c>
       <c r="U10" s="7">
         <f t="shared" si="3"/>
-        <v>0.3359375</v>
+        <v>0.3984375</v>
       </c>
       <c r="V10" s="7">
         <f t="shared" si="2"/>
-        <v>3.148356050744705E-3</v>
+        <v>9.6792975181370089E-4</v>
       </c>
       <c r="W10" s="7">
         <f t="shared" si="4"/>
-        <v>3.6145296199059407E-5</v>
+        <v>1.0084264940128488E-5</v>
       </c>
       <c r="X10" s="7">
         <f t="shared" si="5"/>
-        <v>-1.6247351906757409E-5</v>
+        <v>-8.1499440029630771E-6</v>
       </c>
       <c r="Y10" s="7">
         <f t="shared" si="6"/>
@@ -3039,57 +3036,57 @@
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="F11" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="B11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="F11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
       <c r="J11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K11">
-        <f xml:space="preserve"> K7 + K10^2 / ( PI() * K9 * $C$12 )</f>
-        <v>0.11633747841897502</v>
+        <f xml:space="preserve"> K7 + K10^2 / ( PI() * K9 * $C$22 )</f>
+        <v>0.50964269179464405</v>
       </c>
       <c r="P11" s="7">
         <v>7</v>
       </c>
       <c r="Q11" s="7">
         <f t="shared" si="7"/>
-        <v>0.3359375</v>
+        <v>0.3984375</v>
       </c>
       <c r="R11" s="7">
         <f t="shared" si="0"/>
-        <v>3.148356050744705E-3</v>
+        <v>9.6792975181370089E-4</v>
       </c>
       <c r="S11" s="7">
         <f t="shared" si="8"/>
-        <v>0.34375</v>
+        <v>0.40625</v>
       </c>
       <c r="T11" s="7">
         <f t="shared" si="1"/>
-        <v>-5.1605827437828378E-3</v>
+        <v>-8.4199746806953302E-3</v>
       </c>
       <c r="U11" s="7">
         <f t="shared" si="3"/>
-        <v>0.33984375</v>
+        <v>0.40234375</v>
       </c>
       <c r="V11" s="7">
         <f t="shared" si="2"/>
-        <v>-1.0089381098975503E-3</v>
+        <v>-3.7336157736272968E-3</v>
       </c>
       <c r="W11" s="7">
         <f t="shared" si="4"/>
-        <v>-3.1764964031228784E-6</v>
+        <v>-3.6138777891347884E-6</v>
       </c>
       <c r="X11" s="7">
         <f t="shared" si="5"/>
-        <v>5.2067085994821701E-6</v>
+        <v>3.1436950281386548E-5</v>
       </c>
       <c r="Y11" s="7">
         <f t="shared" si="6"/>
@@ -3098,62 +3095,65 @@
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1">
-        <v>10</v>
+        <v>250</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
       </c>
       <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12">
+        <f xml:space="preserve"> (G4*$C$27 + G9*G13)/3600</f>
+        <v>48547.532757647452</v>
+      </c>
+      <c r="H12" t="s">
         <v>42</v>
       </c>
-      <c r="G12">
-        <f xml:space="preserve"> (G4*$C$29 + G9*G13)/3600</f>
-        <v>21601.37153109724</v>
-      </c>
-      <c r="H12" t="s">
-        <v>43</v>
-      </c>
       <c r="J12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K12">
         <f>K10/K11</f>
-        <v>10.666677730593127</v>
+        <v>6.5472040462851533</v>
       </c>
       <c r="P12" s="7">
         <v>8</v>
       </c>
       <c r="Q12" s="7">
         <f t="shared" si="7"/>
-        <v>0.3359375</v>
+        <v>0.3984375</v>
       </c>
       <c r="R12" s="7">
         <f t="shared" si="0"/>
-        <v>3.148356050744705E-3</v>
+        <v>9.6792975181370089E-4</v>
       </c>
       <c r="S12" s="7">
         <f t="shared" si="8"/>
-        <v>0.33984375</v>
+        <v>0.40234375</v>
       </c>
       <c r="T12" s="7">
         <f t="shared" si="1"/>
-        <v>-1.0089381098975503E-3</v>
+        <v>-3.7336157736272968E-3</v>
       </c>
       <c r="U12" s="7">
         <f t="shared" si="3"/>
-        <v>0.337890625</v>
+        <v>0.400390625</v>
       </c>
       <c r="V12" s="7">
         <f t="shared" si="2"/>
-        <v>1.0689906970746121E-3</v>
+        <v>-1.3847688537725888E-3</v>
       </c>
       <c r="W12" s="7">
         <f t="shared" si="4"/>
-        <v>3.3655633293246553E-6</v>
+        <v>-1.3403589729514449E-6</v>
       </c>
       <c r="X12" s="7">
         <f t="shared" si="5"/>
-        <v>-1.0785454534045238E-6</v>
+        <v>5.1701948352731292E-6</v>
       </c>
       <c r="Y12" s="7">
         <f t="shared" si="6"/>
@@ -3161,60 +3161,66 @@
       </c>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.85</v>
+      </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13">
-        <f xml:space="preserve"> $C$28 / $C$23</f>
-        <v>90.909090909090907</v>
+        <f xml:space="preserve"> $C$26 / $C$20</f>
+        <v>1000</v>
       </c>
       <c r="H13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K13">
-        <f xml:space="preserve"> K5 * K11 * $C$24</f>
-        <v>1379.529819092206</v>
+        <f xml:space="preserve"> K5 * K11 * $C$21</f>
+        <v>2247.5242708143801</v>
       </c>
       <c r="L13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P13" s="7">
         <v>9</v>
       </c>
       <c r="Q13" s="7">
         <f t="shared" si="7"/>
-        <v>0.337890625</v>
+        <v>0.3984375</v>
       </c>
       <c r="R13" s="7">
         <f t="shared" si="0"/>
-        <v>1.0689906970746121E-3</v>
+        <v>9.6792975181370089E-4</v>
       </c>
       <c r="S13" s="7">
         <f t="shared" si="8"/>
-        <v>0.33984375</v>
+        <v>0.400390625</v>
       </c>
       <c r="T13" s="7">
         <f t="shared" si="1"/>
-        <v>-1.0089381098975503E-3</v>
+        <v>-1.3847688537725888E-3</v>
       </c>
       <c r="U13" s="7">
         <f t="shared" si="3"/>
-        <v>0.3388671875</v>
+        <v>0.3994140625</v>
       </c>
       <c r="V13" s="7">
         <f t="shared" si="2"/>
-        <v>2.9848256963116437E-5</v>
+        <v>-2.0890450930222126E-4</v>
       </c>
       <c r="W13" s="7">
         <f t="shared" si="4"/>
-        <v>3.1907509017463989E-8</v>
+        <v>-2.0220488984166199E-7</v>
       </c>
       <c r="X13" s="7">
         <f t="shared" si="5"/>
-        <v>-3.0115043964103091E-8</v>
+        <v>2.8928445789436205E-7</v>
       </c>
       <c r="Y13" s="7">
         <f t="shared" si="6"/>
@@ -3222,45 +3228,46 @@
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B14" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.8</v>
+      </c>
       <c r="P14" s="7">
         <v>10</v>
       </c>
       <c r="Q14" s="7">
         <f t="shared" si="7"/>
-        <v>0.3388671875</v>
+        <v>0.3984375</v>
       </c>
       <c r="R14" s="7">
         <f t="shared" si="0"/>
-        <v>2.9848256963116437E-5</v>
+        <v>9.6792975181370089E-4</v>
       </c>
       <c r="S14" s="7">
         <f t="shared" si="8"/>
-        <v>0.33984375</v>
+        <v>0.3994140625</v>
       </c>
       <c r="T14" s="7">
         <f t="shared" si="1"/>
-        <v>-1.0089381098975503E-3</v>
+        <v>-2.0890450930222126E-4</v>
       </c>
       <c r="U14" s="7">
         <f t="shared" si="3"/>
-        <v>0.33935546875</v>
+        <v>0.39892578125</v>
       </c>
       <c r="V14" s="7">
         <f t="shared" si="2"/>
-        <v>-4.8958924605574383E-4</v>
+        <v>3.7939094077349411E-4</v>
       </c>
       <c r="W14" s="7">
         <f t="shared" si="4"/>
-        <v>-1.4613385622650283E-8</v>
+        <v>3.6722377914325463E-7</v>
       </c>
       <c r="X14" s="7">
         <f t="shared" si="5"/>
-        <v>4.9396524854164887E-7</v>
+        <v>-7.9256478315994871E-8</v>
       </c>
       <c r="Y14" s="7">
         <f t="shared" si="6"/>
@@ -3268,17 +3275,8 @@
       </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="1">
-        <v>280</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>50</v>
+      <c r="J15" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
@@ -3287,35 +3285,35 @@
       </c>
       <c r="Q15" s="7">
         <f t="shared" si="7"/>
-        <v>0.3388671875</v>
+        <v>0.39892578125</v>
       </c>
       <c r="R15" s="7">
         <f t="shared" si="0"/>
-        <v>2.9848256963116437E-5</v>
+        <v>3.7939094077349411E-4</v>
       </c>
       <c r="S15" s="7">
         <f t="shared" si="8"/>
-        <v>0.33935546875</v>
+        <v>0.3994140625</v>
       </c>
       <c r="T15" s="7">
         <f t="shared" si="1"/>
-        <v>-4.8958924605574383E-4</v>
+        <v>-2.0890450930222126E-4</v>
       </c>
       <c r="U15" s="7">
         <f t="shared" si="3"/>
-        <v>0.339111328125</v>
+        <v>0.399169921875</v>
       </c>
       <c r="V15" s="7">
         <f t="shared" si="2"/>
-        <v>-2.2988159805553687E-4</v>
+        <v>8.521285089430064E-5</v>
       </c>
       <c r="W15" s="7">
         <f t="shared" si="4"/>
-        <v>-6.8615650098535127E-9</v>
+        <v>3.2328983666780196E-8</v>
       </c>
       <c r="X15" s="7">
         <f t="shared" si="5"/>
-        <v>1.1254755827409984E-7</v>
+        <v>-1.7801348802317221E-8</v>
       </c>
       <c r="Y15" s="7">
         <f t="shared" si="6"/>
@@ -3323,56 +3321,55 @@
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0.85</v>
-      </c>
+      <c r="B16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
       <c r="J16" t="s">
+        <v>50</v>
+      </c>
+      <c r="K16">
+        <f xml:space="preserve"> (90 - $C$32) / 180 * PI()</f>
+        <v>1.48352986419518</v>
+      </c>
+      <c r="L16" t="s">
         <v>51</v>
-      </c>
-      <c r="K16">
-        <f xml:space="preserve"> (90 - $C$34) / 180 * PI()</f>
-        <v>1.48352986419518</v>
-      </c>
-      <c r="L16" t="s">
-        <v>52</v>
       </c>
       <c r="P16" s="7">
         <v>12</v>
       </c>
       <c r="Q16" s="7">
         <f t="shared" si="7"/>
-        <v>0.3388671875</v>
+        <v>0.399169921875</v>
       </c>
       <c r="R16" s="7">
         <f t="shared" si="0"/>
-        <v>2.9848256963116437E-5</v>
+        <v>8.521285089430064E-5</v>
       </c>
       <c r="S16" s="7">
         <f t="shared" si="8"/>
-        <v>0.339111328125</v>
+        <v>0.3994140625</v>
       </c>
       <c r="T16" s="7">
         <f t="shared" si="1"/>
-        <v>-2.2988159805553687E-4</v>
+        <v>-2.0890450930222126E-4</v>
       </c>
       <c r="U16" s="7">
         <f t="shared" si="3"/>
-        <v>0.3389892578125</v>
+        <v>0.3992919921875</v>
       </c>
       <c r="V16" s="7">
         <f t="shared" si="2"/>
-        <v>-1.0001944938237139E-4</v>
+        <v>-6.1853413518997424E-5</v>
       </c>
       <c r="W16" s="7">
         <f t="shared" si="4"/>
-        <v>-2.9854062264744391E-9</v>
+        <v>-5.2707057034978467E-9</v>
       </c>
       <c r="X16" s="7">
         <f t="shared" si="5"/>
-        <v>2.2992630860654416E-8</v>
+        <v>1.2921456999853537E-8</v>
       </c>
       <c r="Y16" s="7">
         <f t="shared" si="6"/>
@@ -3380,56 +3377,59 @@
       </c>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0.8</v>
+      <c r="B17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1500</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="J17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K17">
         <f xml:space="preserve"> K13 / $C$6</f>
-        <v>1379.529819092206</v>
+        <v>2247.5242708143801</v>
       </c>
       <c r="L17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P17" s="7">
         <v>13</v>
       </c>
       <c r="Q17" s="7">
         <f t="shared" si="7"/>
-        <v>0.3388671875</v>
+        <v>0.399169921875</v>
       </c>
       <c r="R17" s="7">
         <f t="shared" si="0"/>
-        <v>2.9848256963116437E-5</v>
+        <v>8.521285089430064E-5</v>
       </c>
       <c r="S17" s="7">
         <f t="shared" si="8"/>
-        <v>0.3389892578125</v>
+        <v>0.3992919921875</v>
       </c>
       <c r="T17" s="7">
         <f t="shared" si="1"/>
-        <v>-1.0001944938237139E-4</v>
+        <v>-6.1853413518997424E-5</v>
       </c>
       <c r="U17" s="7">
         <f t="shared" si="3"/>
-        <v>0.33892822265625</v>
+        <v>0.39923095703125</v>
       </c>
       <c r="V17" s="7">
         <f t="shared" si="2"/>
-        <v>-3.5086291288954907E-5</v>
+        <v>1.1677821747602124E-5</v>
       </c>
       <c r="W17" s="7">
         <f t="shared" si="4"/>
-        <v>-1.04726463827548E-9</v>
+        <v>9.9510048334864102E-10</v>
       </c>
       <c r="X17" s="7">
         <f t="shared" si="5"/>
-        <v>3.5093115355907638E-9</v>
+        <v>-7.223131375555753E-10</v>
       </c>
       <c r="Y17" s="7">
         <f t="shared" si="6"/>
@@ -3437,50 +3437,59 @@
       </c>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
       <c r="J18" t="s">
+        <v>52</v>
+      </c>
+      <c r="K18">
+        <f xml:space="preserve"> PI() * $C$20 / ($C$19 * $C$23)</f>
+        <v>94.247779607693786</v>
+      </c>
+      <c r="L18" t="s">
         <v>53</v>
-      </c>
-      <c r="K18">
-        <f xml:space="preserve"> PI() * $C$23 / ($C$22 * $C$25)</f>
-        <v>191.98621771937624</v>
-      </c>
-      <c r="L18" t="s">
-        <v>54</v>
       </c>
       <c r="P18" s="7">
         <v>14</v>
       </c>
       <c r="Q18" s="7">
         <f t="shared" si="7"/>
-        <v>0.3388671875</v>
+        <v>0.39923095703125</v>
       </c>
       <c r="R18" s="7">
         <f t="shared" si="0"/>
-        <v>2.9848256963116437E-5</v>
+        <v>1.1677821747602124E-5</v>
       </c>
       <c r="S18" s="7">
         <f t="shared" si="8"/>
-        <v>0.33892822265625</v>
+        <v>0.3992919921875</v>
       </c>
       <c r="T18" s="7">
         <f t="shared" si="1"/>
-        <v>-3.5086291288954907E-5</v>
+        <v>-6.1853413518997424E-5</v>
       </c>
       <c r="U18" s="7">
         <f t="shared" si="3"/>
-        <v>0.338897705078125</v>
+        <v>0.399261474609375</v>
       </c>
       <c r="V18" s="7">
         <f t="shared" si="2"/>
-        <v>-2.6191909791029033E-6</v>
+        <v>-2.5088270013018388E-5</v>
       </c>
       <c r="W18" s="7">
         <f t="shared" si="4"/>
-        <v>-7.8178285379739989E-11</v>
+        <v>-2.9297634516774035E-10</v>
       </c>
       <c r="X18" s="7">
         <f t="shared" si="5"/>
-        <v>9.1897697634207475E-11</v>
+        <v>1.5517951395914892E-9</v>
       </c>
       <c r="Y18" s="7">
         <f t="shared" si="6"/>
@@ -3488,52 +3497,56 @@
       </c>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B19" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
       <c r="J19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K19">
-        <f xml:space="preserve"> $C$23 * COS(K16) / (K18 * $C$22)</f>
-        <v>2.7742534554270872E-2</v>
+        <f xml:space="preserve"> $C$20 * COS(K16) / (K18 * $C$19)</f>
+        <v>2.7742534554270875E-2</v>
       </c>
       <c r="P19" s="7">
         <v>15</v>
       </c>
       <c r="Q19" s="7">
         <f t="shared" si="7"/>
-        <v>0.3388671875</v>
+        <v>0.39923095703125</v>
       </c>
       <c r="R19" s="7">
         <f t="shared" si="0"/>
-        <v>2.9848256963116437E-5</v>
+        <v>1.1677821747602124E-5</v>
       </c>
       <c r="S19" s="7">
         <f t="shared" si="8"/>
-        <v>0.338897705078125</v>
+        <v>0.399261474609375</v>
       </c>
       <c r="T19" s="7">
         <f t="shared" si="1"/>
-        <v>-2.6191909791029033E-6</v>
+        <v>-2.5088270013018388E-5</v>
       </c>
       <c r="U19" s="7">
         <f t="shared" si="3"/>
-        <v>0.3388824462890625</v>
+        <v>0.3992462158203125</v>
       </c>
       <c r="V19" s="7">
         <f t="shared" si="2"/>
-        <v>1.361448953218769E-5</v>
+        <v>-6.7053426779928316E-6</v>
       </c>
       <c r="W19" s="7">
         <f t="shared" si="4"/>
-        <v>4.0636878197839709E-10</v>
+        <v>-7.8303796550189359E-11</v>
       </c>
       <c r="X19" s="7">
         <f t="shared" si="5"/>
-        <v>-3.5658948167796905E-11</v>
+        <v>1.6822544763529998E-10</v>
       </c>
       <c r="Y19" s="7">
         <f t="shared" si="6"/>
@@ -3541,56 +3554,56 @@
       </c>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B20" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="2">
-        <v>1500</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>14</v>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="1">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
       </c>
       <c r="J20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K20">
-        <f xml:space="preserve"> K17 / ( $C$32 * PI() * $C$22^2 * K18^2 * $C$22^2)</f>
-        <v>1.4822961742621928E-2</v>
+        <f xml:space="preserve"> K17 / ( $C$30 * PI() * $C$19^2 * K18^2 * $C$19^2)</f>
+        <v>6.5747035292173767E-2</v>
       </c>
       <c r="P20" s="7">
         <v>16</v>
       </c>
       <c r="Q20" s="7">
         <f t="shared" si="7"/>
-        <v>0.3388824462890625</v>
+        <v>0.39923095703125</v>
       </c>
       <c r="R20" s="7">
         <f t="shared" si="0"/>
-        <v>1.361448953218769E-5</v>
+        <v>1.1677821747602124E-5</v>
       </c>
       <c r="S20" s="7">
         <f t="shared" si="8"/>
-        <v>0.338897705078125</v>
+        <v>0.3992462158203125</v>
       </c>
       <c r="T20" s="7">
         <f t="shared" si="1"/>
-        <v>-2.6191909791029033E-6</v>
+        <v>-6.7053426779928316E-6</v>
       </c>
       <c r="U20" s="7">
         <f t="shared" si="3"/>
-        <v>0.33889007568359375</v>
+        <v>0.39923858642578125</v>
       </c>
       <c r="V20" s="7">
         <f t="shared" si="2"/>
-        <v>5.4976384123439637E-6</v>
+        <v>2.4862098968458923E-6</v>
       </c>
       <c r="W20" s="7">
         <f t="shared" si="4"/>
-        <v>7.4847540616609852E-11</v>
+        <v>2.9033516002490595E-11</v>
       </c>
       <c r="X20" s="7">
         <f t="shared" si="5"/>
-        <v>-1.4399364935980917E-11</v>
+        <v>-1.6670889327768917E-11</v>
       </c>
       <c r="Y20" s="7">
         <f t="shared" si="6"/>
@@ -3599,16 +3612,16 @@
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1">
-        <v>1.2</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K21" s="1">
         <v>1.2E-2</v>
@@ -3618,35 +3631,35 @@
       </c>
       <c r="Q21" s="7">
         <f t="shared" si="7"/>
-        <v>0.33889007568359375</v>
+        <v>0.39923858642578125</v>
       </c>
       <c r="R21" s="7">
         <f t="shared" si="0"/>
-        <v>5.4976384123439637E-6</v>
+        <v>2.4862098968458923E-6</v>
       </c>
       <c r="S21" s="7">
         <f t="shared" si="8"/>
-        <v>0.338897705078125</v>
+        <v>0.3992462158203125</v>
       </c>
       <c r="T21" s="7">
         <f t="shared" si="1"/>
-        <v>-2.6191909791029033E-6</v>
+        <v>-6.7053426779928316E-6</v>
       </c>
       <c r="U21" s="7">
         <f t="shared" si="3"/>
-        <v>0.33889389038085938</v>
+        <v>0.39924240112304688</v>
       </c>
       <c r="V21" s="7">
         <f t="shared" si="2"/>
-        <v>1.4392210006541895E-6</v>
+        <v>-2.1095737998688691E-6</v>
       </c>
       <c r="W21" s="7">
         <f t="shared" si="4"/>
-        <v>7.9123166570485882E-12</v>
+        <v>-5.2448432593607784E-12</v>
       </c>
       <c r="X21" s="7">
         <f t="shared" si="5"/>
-        <v>-3.7695946618489064E-12</v>
+        <v>1.4145415232636236E-11</v>
       </c>
       <c r="Y21" s="7">
         <f t="shared" si="6"/>
@@ -3655,58 +3668,55 @@
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="D22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K22">
-        <f xml:space="preserve"> ($C$8 * $K$21 / 8) * (1 + 4.65 * K19^2) * ( PI() * $C$32 * K18^3 * C22^5)</f>
-        <v>3146.9858091218234</v>
+        <f xml:space="preserve"> ($C$8 * $K$21 / 8) * (1 + 4.65 * K19^2) * ( PI() * $C$30 * K18^3 * C19^5)</f>
+        <v>630.50053776545394</v>
       </c>
       <c r="L22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P22" s="7">
         <v>18</v>
       </c>
       <c r="Q22" s="7">
         <f t="shared" si="7"/>
-        <v>0.33889389038085938</v>
+        <v>0.39923858642578125</v>
       </c>
       <c r="R22" s="7">
         <f t="shared" si="0"/>
-        <v>1.4392210006541895E-6</v>
+        <v>2.4862098968458923E-6</v>
       </c>
       <c r="S22" s="7">
         <f t="shared" si="8"/>
-        <v>0.338897705078125</v>
+        <v>0.39924240112304688</v>
       </c>
       <c r="T22" s="7">
         <f t="shared" si="1"/>
-        <v>-2.6191909791029033E-6</v>
+        <v>-2.1095737998688691E-6</v>
       </c>
       <c r="U22" s="7">
         <f t="shared" si="3"/>
-        <v>0.33889579772949219</v>
+        <v>0.39924049377441406</v>
       </c>
       <c r="V22" s="7">
         <f t="shared" si="2"/>
-        <v>-5.8998566820900322E-7</v>
+        <v>1.883161961369062E-7</v>
       </c>
       <c r="W22" s="7">
         <f t="shared" si="4"/>
-        <v>-8.4911976377139224E-13</v>
+        <v>4.6819359057194836E-13</v>
       </c>
       <c r="X22" s="7">
         <f t="shared" si="5"/>
-        <v>1.5452851399730198E-12</v>
+        <v>-3.9726691346138447E-13</v>
       </c>
       <c r="Y22" s="7">
         <f t="shared" si="6"/>
@@ -3715,55 +3725,52 @@
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1">
-        <v>55</v>
-      </c>
-      <c r="D23" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K23" s="4">
         <f>U34</f>
-        <v>0.338895243126899</v>
+        <v>0.39924064977094531</v>
       </c>
       <c r="P23" s="7">
         <v>19</v>
       </c>
       <c r="Q23" s="7">
         <f t="shared" si="7"/>
-        <v>0.33889389038085938</v>
+        <v>0.39924049377441406</v>
       </c>
       <c r="R23" s="7">
         <f t="shared" si="0"/>
-        <v>1.4392210006541895E-6</v>
+        <v>1.883161961369062E-7</v>
       </c>
       <c r="S23" s="7">
         <f t="shared" si="8"/>
-        <v>0.33889579772949219</v>
+        <v>0.39924240112304688</v>
       </c>
       <c r="T23" s="7">
         <f t="shared" si="1"/>
-        <v>-5.8998566820900322E-7</v>
+        <v>-2.1095737998688691E-6</v>
       </c>
       <c r="U23" s="7">
         <f t="shared" si="3"/>
-        <v>0.33889484405517578</v>
+        <v>0.39924144744873047</v>
       </c>
       <c r="V23" s="7">
         <f t="shared" si="2"/>
-        <v>4.2461749649724823E-7</v>
+        <v>-9.6062926496776058E-7</v>
       </c>
       <c r="W23" s="7">
         <f t="shared" si="4"/>
-        <v>6.1111841820404638E-13</v>
+        <v>-1.8090204907652084E-13</v>
       </c>
       <c r="X23" s="7">
         <f t="shared" si="5"/>
-        <v>-2.5051823740416309E-13</v>
+        <v>2.0265183287632772E-12</v>
       </c>
       <c r="Y23" s="7">
         <f t="shared" si="6"/>
@@ -3771,59 +3778,50 @@
       </c>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="1">
-        <v>6.4</v>
-      </c>
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
       <c r="J24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K24">
-        <f xml:space="preserve"> K18 * $C$22 * K23 - $C$23 * SIN(K16)</f>
-        <v>3.766185942873598</v>
+        <f xml:space="preserve"> K18 * $C$19 * K23 - $C$20 * SIN(K16)</f>
+        <v>7.7417038272921488</v>
       </c>
       <c r="L24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P24" s="7">
         <v>20</v>
       </c>
       <c r="Q24" s="7">
         <f t="shared" si="7"/>
-        <v>0.33889484405517578</v>
+        <v>0.39924049377441406</v>
       </c>
       <c r="R24" s="7">
         <f t="shared" si="0"/>
-        <v>4.2461749649724823E-7</v>
+        <v>1.883161961369062E-7</v>
       </c>
       <c r="S24" s="7">
         <f t="shared" si="8"/>
-        <v>0.33889579772949219</v>
+        <v>0.39924144744873047</v>
       </c>
       <c r="T24" s="7">
         <f t="shared" si="1"/>
-        <v>-5.8998566820900322E-7</v>
+        <v>-9.6062926496776058E-7</v>
       </c>
       <c r="U24" s="7">
         <f t="shared" si="3"/>
-        <v>0.33889532089233398</v>
+        <v>0.39924097061157227</v>
       </c>
       <c r="V24" s="7">
         <f t="shared" si="2"/>
-        <v>-8.2684128266397039E-8</v>
+        <v>-3.8615665021168866E-7</v>
       </c>
       <c r="W24" s="7">
         <f t="shared" si="4"/>
-        <v>-3.5109127544534869E-14</v>
+        <v>-7.2719551480835047E-14</v>
       </c>
       <c r="X24" s="7">
         <f t="shared" si="5"/>
-        <v>4.8782450665529188E-14</v>
+        <v>3.7095337905526712E-13</v>
       </c>
       <c r="Y24" s="7">
         <f t="shared" si="6"/>
@@ -3831,53 +3829,52 @@
       </c>
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+      <c r="B25" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
       <c r="J25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K25">
-        <f xml:space="preserve"> 1/$C$9 - K22 * SQRT( (2*$C$32*PI()*$C$22^2) / K17^3 )</f>
-        <v>1.1799780884059028</v>
+        <f xml:space="preserve"> 1/$C$9 - K22 * SQRT( (2*$C$30*PI()*$C$19^2) / K17^3 )</f>
+        <v>1.3169165958189717</v>
       </c>
       <c r="P25" s="7">
         <v>21</v>
       </c>
       <c r="Q25" s="7">
         <f t="shared" si="7"/>
-        <v>0.33889484405517578</v>
+        <v>0.39924049377441406</v>
       </c>
       <c r="R25" s="7">
         <f t="shared" si="0"/>
-        <v>4.2461749649724823E-7</v>
+        <v>1.883161961369062E-7</v>
       </c>
       <c r="S25" s="7">
         <f t="shared" si="8"/>
-        <v>0.33889532089233398</v>
+        <v>0.39924097061157227</v>
       </c>
       <c r="T25" s="7">
         <f t="shared" si="1"/>
-        <v>-8.2684128266397039E-8</v>
+        <v>-3.8615665021168866E-7</v>
       </c>
       <c r="U25" s="7">
         <f t="shared" si="3"/>
-        <v>0.33889508247375488</v>
+        <v>0.39924073219299316</v>
       </c>
       <c r="V25" s="7">
         <f t="shared" si="2"/>
-        <v>1.7096667348504013E-7</v>
+        <v>-9.8920255986456596E-8</v>
       </c>
       <c r="W25" s="7">
         <f t="shared" si="4"/>
-        <v>7.2595440879680204E-14</v>
+        <v>-1.8628286328258529E-14</v>
       </c>
       <c r="X25" s="7">
         <f t="shared" si="5"/>
-        <v>-1.413623035971628E-14</v>
+        <v>3.8198714689812819E-14</v>
       </c>
       <c r="Y25" s="7">
         <f t="shared" si="6"/>
@@ -3885,8 +3882,17 @@
       </c>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="1">
+        <v>30000</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
       <c r="J26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K26" s="1">
         <v>1.1499999999999999</v>
@@ -3896,35 +3902,35 @@
       </c>
       <c r="Q26" s="7">
         <f t="shared" si="7"/>
-        <v>0.33889508247375488</v>
+        <v>0.39924049377441406</v>
       </c>
       <c r="R26" s="7">
         <f t="shared" si="0"/>
-        <v>1.7096667348504013E-7</v>
+        <v>1.883161961369062E-7</v>
       </c>
       <c r="S26" s="7">
         <f t="shared" si="8"/>
-        <v>0.33889532089233398</v>
+        <v>0.39924073219299316</v>
       </c>
       <c r="T26" s="7">
         <f t="shared" si="1"/>
-        <v>-8.2684128266397039E-8</v>
+        <v>-9.8920255986456596E-8</v>
       </c>
       <c r="U26" s="7">
         <f t="shared" si="3"/>
-        <v>0.33889520168304443</v>
+        <v>0.39924061298370361</v>
       </c>
       <c r="V26" s="7">
         <f t="shared" si="2"/>
-        <v>4.4141269972541863E-8</v>
+        <v>4.4697962831019566E-8</v>
       </c>
       <c r="W26" s="7">
         <f t="shared" si="4"/>
-        <v>7.5466860906105707E-15</v>
+        <v>8.4173503354064244E-15</v>
       </c>
       <c r="X26" s="7">
         <f t="shared" si="5"/>
-        <v>-3.6497824282513118E-15</v>
+        <v>-4.421533925317578E-15</v>
       </c>
       <c r="Y26" s="7">
         <f t="shared" si="6"/>
@@ -3932,52 +3938,56 @@
       </c>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B27" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1">
+        <v>240</v>
+      </c>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
       <c r="J27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K27">
-        <f xml:space="preserve"> 1/$C$37 * LN( EXP($C$37 * K25) + EXP($C$37 * K26) )</f>
-        <v>1.1913562192675804</v>
+        <f xml:space="preserve"> 1/$C$35 * LN( EXP($C$35 * K25) + EXP($C$35 * K26) )</f>
+        <v>1.3171387742437404</v>
       </c>
       <c r="P27" s="7">
         <v>23</v>
       </c>
       <c r="Q27" s="7">
         <f t="shared" si="7"/>
-        <v>0.33889520168304443</v>
+        <v>0.39924061298370361</v>
       </c>
       <c r="R27" s="7">
         <f t="shared" si="0"/>
-        <v>4.4141269972541863E-8</v>
+        <v>4.4697962831019566E-8</v>
       </c>
       <c r="S27" s="7">
         <f t="shared" si="8"/>
-        <v>0.33889532089233398</v>
+        <v>0.39924073219299316</v>
       </c>
       <c r="T27" s="7">
         <f t="shared" si="1"/>
-        <v>-8.2684128266397039E-8</v>
+        <v>-9.8920255986456596E-8</v>
       </c>
       <c r="U27" s="7">
         <f t="shared" si="3"/>
-        <v>0.33889526128768921</v>
+        <v>0.39924067258834839</v>
       </c>
       <c r="V27" s="7">
         <f t="shared" si="2"/>
-        <v>-1.9271429840816978E-8</v>
+        <v>-2.711114838183093E-8</v>
       </c>
       <c r="W27" s="7">
         <f t="shared" si="4"/>
-        <v>-8.5066538736040171E-16</v>
+        <v>-1.2118131026773352E-15</v>
       </c>
       <c r="X27" s="7">
         <f t="shared" si="5"/>
-        <v>1.5934413768349824E-15</v>
+        <v>2.6818417380175242E-15</v>
       </c>
       <c r="Y27" s="7">
         <f t="shared" si="6"/>
@@ -3985,49 +3995,40 @@
       </c>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="1">
-        <v>5000</v>
-      </c>
-      <c r="D28" t="s">
-        <v>16</v>
-      </c>
       <c r="P28" s="7">
         <v>24</v>
       </c>
       <c r="Q28" s="7">
         <f t="shared" si="7"/>
-        <v>0.33889520168304443</v>
+        <v>0.39924061298370361</v>
       </c>
       <c r="R28" s="7">
         <f t="shared" si="0"/>
-        <v>4.4141269972541863E-8</v>
+        <v>4.4697962831019566E-8</v>
       </c>
       <c r="S28" s="7">
         <f t="shared" si="8"/>
-        <v>0.33889526128768921</v>
+        <v>0.39924067258834839</v>
       </c>
       <c r="T28" s="7">
         <f t="shared" si="1"/>
-        <v>-1.9271429840816978E-8</v>
+        <v>-2.711114838183093E-8</v>
       </c>
       <c r="U28" s="7">
         <f t="shared" si="3"/>
-        <v>0.33889523148536682</v>
+        <v>0.399240642786026</v>
       </c>
       <c r="V28" s="7">
         <f t="shared" si="2"/>
-        <v>1.2434919871573413E-8</v>
+        <v>8.7934067805051086E-9</v>
       </c>
       <c r="W28" s="7">
         <f t="shared" si="4"/>
-        <v>5.4889315513804766E-16</v>
+        <v>3.9304736943305279E-16</v>
       </c>
       <c r="X28" s="7">
         <f t="shared" si="5"/>
-        <v>-2.396386858812079E-16</v>
+        <v>-2.3839935600807219E-16</v>
       </c>
       <c r="Y28" s="7">
         <f t="shared" si="6"/>
@@ -4035,49 +4036,45 @@
       </c>
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="1">
-        <v>240</v>
-      </c>
-      <c r="D29" t="s">
-        <v>26</v>
-      </c>
+      <c r="B29" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
       <c r="P29" s="7">
         <v>25</v>
       </c>
       <c r="Q29" s="7">
         <f t="shared" si="7"/>
-        <v>0.33889523148536682</v>
+        <v>0.399240642786026</v>
       </c>
       <c r="R29" s="7">
         <f t="shared" si="0"/>
-        <v>1.2434919871573413E-8</v>
+        <v>8.7934067805051086E-9</v>
       </c>
       <c r="S29" s="7">
         <f t="shared" si="8"/>
-        <v>0.33889526128768921</v>
+        <v>0.39924067258834839</v>
       </c>
       <c r="T29" s="7">
         <f t="shared" si="1"/>
-        <v>-1.9271429840816978E-8</v>
+        <v>-2.711114838183093E-8</v>
       </c>
       <c r="U29" s="7">
         <f t="shared" si="3"/>
-        <v>0.33889524638652802</v>
+        <v>0.39924065768718719</v>
       </c>
       <c r="V29" s="7">
         <f t="shared" si="2"/>
-        <v>-3.4182550123773581E-9</v>
+        <v>-9.1588708839296373E-9</v>
       </c>
       <c r="W29" s="7">
         <f t="shared" si="4"/>
-        <v>-4.2505727179516634E-17</v>
+        <v>-8.053767733251769E-17</v>
       </c>
       <c r="X29" s="7">
         <f t="shared" si="5"/>
-        <v>6.5874661649051227E-17</v>
+        <v>2.483075075442474E-16</v>
       </c>
       <c r="Y29" s="7">
         <f t="shared" si="6"/>
@@ -4085,40 +4082,49 @@
       </c>
     </row>
     <row r="30" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="D30" t="s">
+        <v>27</v>
+      </c>
       <c r="P30" s="7">
         <v>26</v>
       </c>
       <c r="Q30" s="7">
         <f t="shared" si="7"/>
-        <v>0.33889523148536682</v>
+        <v>0.399240642786026</v>
       </c>
       <c r="R30" s="7">
         <f t="shared" si="0"/>
-        <v>1.2434919871573413E-8</v>
+        <v>8.7934067805051086E-9</v>
       </c>
       <c r="S30" s="7">
         <f t="shared" si="8"/>
-        <v>0.33889524638652802</v>
+        <v>0.39924065768718719</v>
       </c>
       <c r="T30" s="7">
         <f t="shared" si="1"/>
-        <v>-3.4182550123773581E-9</v>
+        <v>-9.1588708839296373E-9</v>
       </c>
       <c r="U30" s="7">
         <f t="shared" si="3"/>
-        <v>0.33889523893594742</v>
+        <v>0.3992406502366066</v>
       </c>
       <c r="V30" s="7">
         <f t="shared" si="2"/>
-        <v>4.5083324295980276E-9</v>
+        <v>-1.827321072234156E-10</v>
       </c>
       <c r="W30" s="7">
         <f t="shared" si="4"/>
-        <v>5.6060752516467353E-17</v>
+        <v>-1.6068377506743692E-18</v>
       </c>
       <c r="X30" s="7">
         <f t="shared" si="5"/>
-        <v>-1.5410629924936851E-17</v>
+        <v>1.6736197764076497E-18</v>
       </c>
       <c r="Y30" s="7">
         <f t="shared" si="6"/>
@@ -4126,45 +4132,49 @@
       </c>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B31" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="B31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="1">
+        <v>9.81</v>
+      </c>
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
       <c r="P31" s="7">
         <v>27</v>
       </c>
       <c r="Q31" s="7">
         <f t="shared" si="7"/>
-        <v>0.33889523893594742</v>
+        <v>0.399240642786026</v>
       </c>
       <c r="R31" s="7">
         <f t="shared" si="0"/>
-        <v>4.5083324295980276E-9</v>
+        <v>8.7934067805051086E-9</v>
       </c>
       <c r="S31" s="7">
         <f t="shared" si="8"/>
-        <v>0.33889524638652802</v>
+        <v>0.3992406502366066</v>
       </c>
       <c r="T31" s="7">
         <f t="shared" si="1"/>
-        <v>-3.4182550123773581E-9</v>
+        <v>-1.827321072234156E-10</v>
       </c>
       <c r="U31" s="7">
         <f t="shared" si="3"/>
-        <v>0.33889524266123772</v>
+        <v>0.3992406465113163</v>
       </c>
       <c r="V31" s="7">
         <f t="shared" si="2"/>
-        <v>5.4503868085475915E-10</v>
+        <v>4.3053373088852709E-9</v>
       </c>
       <c r="W31" s="7">
         <f t="shared" si="4"/>
-        <v>2.4572155602828403E-18</v>
+        <v>3.7858582284313358E-17</v>
       </c>
       <c r="X31" s="7">
         <f t="shared" si="5"/>
-        <v>-1.8630812027713237E-18</v>
+        <v>-7.8672335876019487E-19</v>
       </c>
       <c r="Y31" s="7">
         <f t="shared" si="6"/>
@@ -4173,48 +4183,48 @@
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="C32" s="1">
-        <v>1.2250000000000001</v>
+        <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="P32" s="7">
         <v>28</v>
       </c>
       <c r="Q32" s="7">
         <f t="shared" si="7"/>
-        <v>0.33889524266123772</v>
+        <v>0.3992406465113163</v>
       </c>
       <c r="R32" s="7">
         <f t="shared" si="0"/>
-        <v>5.4503868085475915E-10</v>
+        <v>4.3053373088852709E-9</v>
       </c>
       <c r="S32" s="7">
         <f t="shared" si="8"/>
-        <v>0.33889524638652802</v>
+        <v>0.3992406502366066</v>
       </c>
       <c r="T32" s="7">
         <f t="shared" si="1"/>
-        <v>-3.4182550123773581E-9</v>
+        <v>-1.827321072234156E-10</v>
       </c>
       <c r="U32" s="7">
         <f t="shared" si="3"/>
-        <v>0.33889524452388287</v>
+        <v>0.39924064837396145</v>
       </c>
       <c r="V32" s="7">
         <f t="shared" si="2"/>
-        <v>-1.4366081657612995E-9</v>
+        <v>2.0613026285865033E-9</v>
       </c>
       <c r="W32" s="7">
         <f t="shared" si="4"/>
-        <v>-7.8300701957171383E-19</v>
+        <v>8.874603111756751E-18</v>
       </c>
       <c r="X32" s="7">
         <f t="shared" si="5"/>
-        <v>4.9106930634358044E-18</v>
+        <v>-3.7666617294677733E-19</v>
       </c>
       <c r="Y32" s="7">
         <f t="shared" si="6"/>
@@ -4222,49 +4232,40 @@
       </c>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="1">
-        <v>9.81</v>
-      </c>
-      <c r="D33" t="s">
-        <v>30</v>
-      </c>
       <c r="P33" s="7">
         <v>29</v>
       </c>
       <c r="Q33" s="7">
         <f t="shared" si="7"/>
-        <v>0.33889524266123772</v>
+        <v>0.39924064837396145</v>
       </c>
       <c r="R33" s="7">
         <f t="shared" si="0"/>
-        <v>5.4503868085475915E-10</v>
+        <v>2.0613026285865033E-9</v>
       </c>
       <c r="S33" s="7">
         <f t="shared" si="8"/>
-        <v>0.33889524452388287</v>
+        <v>0.3992406502366066</v>
       </c>
       <c r="T33" s="7">
         <f t="shared" si="1"/>
-        <v>-1.4366081657612995E-9</v>
+        <v>-1.827321072234156E-10</v>
       </c>
       <c r="U33" s="7">
         <f t="shared" si="3"/>
-        <v>0.33889524359256029</v>
+        <v>0.39924064930528402</v>
       </c>
       <c r="V33" s="7">
         <f t="shared" si="2"/>
-        <v>-4.4578474245327016E-10</v>
+        <v>9.3928526068154383E-10</v>
       </c>
       <c r="W33" s="7">
         <f t="shared" si="4"/>
-        <v>-2.4296992797190891E-19</v>
+        <v>1.9361511768354252E-18</v>
       </c>
       <c r="X33" s="7">
         <f t="shared" si="5"/>
-        <v>6.4041800118016572E-19</v>
+        <v>-1.7163757496823374E-19</v>
       </c>
       <c r="Y33" s="7">
         <f t="shared" si="6"/>
@@ -4272,85 +4273,73 @@
       </c>
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="1">
-        <v>5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>75</v>
-      </c>
+      <c r="B34" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
       <c r="P34" s="7">
         <v>30</v>
       </c>
       <c r="Q34" s="7">
         <f t="shared" si="7"/>
-        <v>0.33889524266123772</v>
+        <v>0.39924064930528402</v>
       </c>
       <c r="R34" s="7">
         <f t="shared" si="0"/>
-        <v>5.4503868085475915E-10</v>
+        <v>9.3928526068154383E-10</v>
       </c>
       <c r="S34" s="7">
         <f t="shared" si="8"/>
-        <v>0.33889524359256029</v>
+        <v>0.3992406502366066</v>
       </c>
       <c r="T34" s="7">
         <f t="shared" si="1"/>
-        <v>-4.4578474245327016E-10</v>
+        <v>-1.827321072234156E-10</v>
       </c>
       <c r="U34" s="7">
         <f t="shared" si="3"/>
-        <v>0.338895243126899</v>
+        <v>0.39924064977094531</v>
       </c>
       <c r="V34" s="7">
         <f t="shared" si="2"/>
-        <v>4.9626969200744497E-11</v>
+        <v>3.7827657672906412E-10</v>
       </c>
       <c r="W34" s="7">
         <f t="shared" si="4"/>
-        <v>2.7048617827993542E-20</v>
+        <v>3.5530961298268101E-19</v>
       </c>
       <c r="X34" s="7">
         <f t="shared" si="5"/>
-        <v>-2.2122945683890256E-20</v>
+        <v>-6.9123275978961941E-20</v>
       </c>
       <c r="Y34" s="7">
         <f t="shared" si="6"/>
         <v>9.3132257461547852E-10</v>
       </c>
     </row>
-    <row r="36" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B36" s="12" t="s">
+    <row r="35" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="2:25" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>32</v>
-      </c>
-      <c r="C37" s="1">
+      <c r="C35" s="1">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B27:D27"/>
+  <mergeCells count="12">
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B25:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new sheets with BEMT capabilities
</commit_message>
<xml_diff>
--- a/sheets/estimate_energy.xlsx
+++ b/sheets/estimate_energy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfiyandyhr/Github_Repos/MCEVS/sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F775BF2-38C0-7D43-A11A-5AFD4CFC3ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F45C767-03E8-B34A-B411-9DE7A0A1AF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15320" yWindow="740" windowWidth="14920" windowHeight="18900" activeTab="1" xr2:uid="{843CD013-835A-1741-B375-CD508AE79BD2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" activeTab="1" xr2:uid="{843CD013-835A-1741-B375-CD508AE79BD2}"/>
   </bookViews>
   <sheets>
     <sheet name="multirotor_aerofidelity1" sheetId="6" r:id="rId1"/>
@@ -653,27 +653,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -1012,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A2C9A4-014D-1547-9F90-2CE2D6D869E1}">
   <dimension ref="B1:AK104"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1056,11 +1056,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="2:37" x14ac:dyDescent="0.2">
       <c r="AB2" s="12" t="s">
@@ -1068,36 +1068,36 @@
       </c>
     </row>
     <row r="3" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="20" t="s">
         <v>73</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="20" t="s">
         <v>81</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="N3" s="24" t="s">
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="N3" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="R3" s="24" t="s">
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="R3" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="V3" s="24" t="s">
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="V3" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
       <c r="AB3" s="14" t="s">
         <v>63</v>
       </c>
@@ -1148,9 +1148,9 @@
       <c r="J4" t="s">
         <v>87</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="11" t="e">
         <f>MAX(G6,G18,G34,G40)*1000</f>
-        <v>178508.37531883034</v>
+        <v>#REF!</v>
       </c>
       <c r="L4" s="11" t="s">
         <v>29</v>
@@ -1242,9 +1242,9 @@
       <c r="J5" t="s">
         <v>89</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="11" t="e">
         <f>K4/$C$5</f>
-        <v>44627.093829707585</v>
+        <v>#REF!</v>
       </c>
       <c r="L5" s="11" t="s">
         <v>29</v>
@@ -1492,11 +1492,11 @@
       <c r="H8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="J8" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
       <c r="AB8" s="7">
         <v>4</v>
       </c>
@@ -1538,7 +1538,7 @@
       </c>
     </row>
     <row r="9" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="23"/>
@@ -1548,9 +1548,9 @@
       <c r="J9" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="11" t="e">
         <f xml:space="preserve"> (G6*G8 + G18*G19 + G23*G24 + G34*G35 + G40*G42)/3600</f>
-        <v>58.850608823382295</v>
+        <v>#REF!</v>
       </c>
       <c r="L9" s="11" t="s">
         <v>94</v>
@@ -1620,21 +1620,21 @@
       <c r="L10" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="N10" s="22" t="s">
+      <c r="N10" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="R10" s="22" t="s">
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="R10" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
-      <c r="V10" s="22" t="s">
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="V10" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="W10" s="27"/>
-      <c r="X10" s="27"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21"/>
       <c r="AB10" s="7">
         <v>6</v>
       </c>
@@ -1896,11 +1896,11 @@
       </c>
     </row>
     <row r="14" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="F14" t="s">
         <v>101</v>
       </c>
@@ -1971,21 +1971,21 @@
       <c r="H15" t="s">
         <v>14</v>
       </c>
-      <c r="N15" s="22" t="s">
+      <c r="N15" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="R15" s="22" t="s">
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="R15" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="S15" s="27"/>
-      <c r="T15" s="27"/>
-      <c r="V15" s="22" t="s">
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="V15" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="W15" s="27"/>
-      <c r="X15" s="27"/>
+      <c r="W15" s="21"/>
+      <c r="X15" s="21"/>
       <c r="AB15" s="7">
         <v>11</v>
       </c>
@@ -2366,11 +2366,11 @@
       </c>
     </row>
     <row r="20" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
       <c r="N20" s="11" t="s">
         <v>4</v>
       </c>
@@ -2439,7 +2439,7 @@
       <c r="D21" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="20" t="s">
         <v>108</v>
       </c>
       <c r="G21" s="23"/>
@@ -2599,9 +2599,9 @@
       <c r="F23" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="11">
-        <f>$C$5 * G22</f>
-        <v>96.403786262092765</v>
+      <c r="G23" s="11" t="e">
+        <f>#REF! * $C$5 * G22</f>
+        <v>#REF!</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>91</v>
@@ -2677,11 +2677,11 @@
       </c>
     </row>
     <row r="24" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
       <c r="F24" s="18" t="s">
         <v>110</v>
       </c>
@@ -3006,11 +3006,11 @@
       </c>
     </row>
     <row r="29" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
       <c r="F29" t="s">
         <v>99</v>
       </c>
@@ -3169,11 +3169,11 @@
       </c>
     </row>
     <row r="32" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
       <c r="F32" t="s">
         <v>103</v>
       </c>
@@ -3235,9 +3235,9 @@
       <c r="F33" t="s">
         <v>104</v>
       </c>
-      <c r="G33" s="11">
-        <f xml:space="preserve"> 1/1000 * (W21 + W17 * (W26 * W23 + $G$27 * SIN(W16/180*PI())))</f>
-        <v>20.301891897125365</v>
+      <c r="G33" s="11" t="e">
+        <f>#REF! * 1/1000 * (W21 + W17 * (W26 * W23 + $G$27 * SIN(W16/180*PI())))</f>
+        <v>#REF!</v>
       </c>
       <c r="H33" t="s">
         <v>91</v>
@@ -3293,9 +3293,9 @@
       <c r="F34" t="s">
         <v>113</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="11" t="e">
         <f>$C$5*G33</f>
-        <v>81.207567588501462</v>
+        <v>#REF!</v>
       </c>
       <c r="H34" t="s">
         <v>91</v>
@@ -3356,11 +3356,11 @@
       </c>
     </row>
     <row r="36" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
     </row>
     <row r="37" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
@@ -3370,7 +3370,7 @@
         <v>4</v>
       </c>
       <c r="D37"/>
-      <c r="F37" s="22" t="s">
+      <c r="F37" s="20" t="s">
         <v>115</v>
       </c>
       <c r="G37" s="23"/>
@@ -3541,11 +3541,11 @@
       </c>
     </row>
     <row r="41" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
       <c r="F41" t="s">
         <v>30</v>
       </c>
@@ -6078,6 +6078,22 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="R10:T10"/>
+    <mergeCell ref="V10:X10"/>
+    <mergeCell ref="R3:T3"/>
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="R15:T15"/>
     <mergeCell ref="V15:X15"/>
@@ -6088,22 +6104,6 @@
     <mergeCell ref="F26:H26"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="N10:P10"/>
-    <mergeCell ref="R10:T10"/>
-    <mergeCell ref="V10:X10"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6113,8 +6113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7633D22C-2729-244F-93D1-A98029DF7C83}">
   <dimension ref="B1:AK104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6155,11 +6155,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="2:37" x14ac:dyDescent="0.2">
       <c r="AB2" s="5" t="s">
@@ -6167,36 +6167,36 @@
       </c>
     </row>
     <row r="3" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
       <c r="F3" s="25" t="s">
         <v>81</v>
       </c>
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="N3" s="20" t="s">
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="N3" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="R3" s="20" t="s">
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="R3" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="V3" s="20" t="s">
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="V3" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="W3" s="20"/>
-      <c r="X3" s="20"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="27"/>
       <c r="AB3" s="6" t="s">
         <v>63</v>
       </c>
@@ -6752,11 +6752,11 @@
       </c>
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
-      <c r="J10" s="24" t="s">
+      <c r="J10" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
       <c r="N10" t="s">
         <v>128</v>
       </c>
@@ -6819,7 +6819,7 @@
       </c>
     </row>
     <row r="11" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="23"/>
@@ -7220,11 +7220,11 @@
       </c>
     </row>
     <row r="16" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
       <c r="F16" t="s">
         <v>103</v>
       </c>
@@ -7975,11 +7975,11 @@
       </c>
     </row>
     <row r="25" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
       <c r="F25" s="3"/>
       <c r="K25" s="1">
         <v>20</v>
@@ -8578,11 +8578,11 @@
       </c>
     </row>
     <row r="35" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
       <c r="F35" t="s">
         <v>114</v>
       </c>
@@ -8613,11 +8613,11 @@
       </c>
     </row>
     <row r="38" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
       <c r="F38" t="s">
         <v>117</v>
       </c>
@@ -8878,11 +8878,11 @@
       </c>
     </row>
     <row r="43" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
       <c r="AB43" s="7">
         <v>4</v>
       </c>
@@ -9112,11 +9112,11 @@
       </c>
     </row>
     <row r="48" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
       <c r="AB48" s="7">
         <v>9</v>
       </c>
@@ -9296,11 +9296,11 @@
       </c>
     </row>
     <row r="52" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
       <c r="AB52" s="7">
         <v>13</v>
       </c>
@@ -9430,11 +9430,11 @@
       </c>
     </row>
     <row r="55" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
       <c r="AB55" s="7">
         <v>16</v>
       </c>
@@ -9665,11 +9665,11 @@
       </c>
     </row>
     <row r="60" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
       <c r="AB60" s="7">
         <v>21</v>
       </c>
@@ -11421,11 +11421,17 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="N3:P3"/>
     <mergeCell ref="V3:X3"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="J10:L10"/>
@@ -11434,17 +11440,11 @@
     <mergeCell ref="R14:T14"/>
     <mergeCell ref="V14:X14"/>
     <mergeCell ref="R3:T3"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11498,11 +11498,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="2:37" x14ac:dyDescent="0.2">
       <c r="AB2" s="12" t="s">
@@ -11510,36 +11510,36 @@
       </c>
     </row>
     <row r="3" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="20" t="s">
         <v>73</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="20" t="s">
         <v>81</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="N3" s="24" t="s">
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="N3" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="R3" s="24" t="s">
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="R3" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="V3" s="24" t="s">
+      <c r="S3" s="22"/>
+      <c r="T3" s="22"/>
+      <c r="V3" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="22"/>
       <c r="AB3" s="14" t="s">
         <v>63</v>
       </c>
@@ -11937,11 +11937,11 @@
       <c r="H8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="J8" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
       <c r="N8" s="11" t="s">
         <v>60</v>
       </c>
@@ -12013,7 +12013,7 @@
       </c>
     </row>
     <row r="9" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="23"/>
@@ -12152,21 +12152,21 @@
       <c r="H11" t="s">
         <v>16</v>
       </c>
-      <c r="N11" s="22" t="s">
+      <c r="N11" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="R11" s="22" t="s">
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="R11" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
-      <c r="V11" s="22" t="s">
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="V11" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="W11" s="27"/>
-      <c r="X11" s="27"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="21"/>
       <c r="AB11" s="7">
         <v>7</v>
       </c>
@@ -12371,11 +12371,11 @@
       </c>
     </row>
     <row r="14" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="F14" t="s">
         <v>101</v>
       </c>
@@ -12506,21 +12506,21 @@
       <c r="H16" t="s">
         <v>62</v>
       </c>
-      <c r="N16" s="22" t="s">
+      <c r="N16" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="R16" s="22" t="s">
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="R16" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="S16" s="27"/>
-      <c r="T16" s="27"/>
-      <c r="V16" s="22" t="s">
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="V16" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="W16" s="27"/>
-      <c r="X16" s="27"/>
+      <c r="W16" s="21"/>
+      <c r="X16" s="21"/>
       <c r="AB16" s="7">
         <v>12</v>
       </c>
@@ -12820,11 +12820,11 @@
       </c>
     </row>
     <row r="20" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
       <c r="N20" s="11" t="s">
         <v>45</v>
       </c>
@@ -12896,7 +12896,7 @@
       <c r="D21" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="20" t="s">
         <v>108</v>
       </c>
       <c r="G21" s="23"/>
@@ -13122,11 +13122,11 @@
       </c>
     </row>
     <row r="24" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
       <c r="F24" s="18" t="s">
         <v>110</v>
       </c>
@@ -13481,11 +13481,11 @@
       </c>
     </row>
     <row r="29" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
       <c r="F29" t="s">
         <v>99</v>
       </c>
@@ -13812,7 +13812,7 @@
       </c>
     </row>
     <row r="37" spans="6:37" x14ac:dyDescent="0.2">
-      <c r="F37" s="22" t="s">
+      <c r="F37" s="20" t="s">
         <v>115</v>
       </c>
       <c r="G37" s="23"/>
@@ -16478,16 +16478,11 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="N16:P16"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="V16:X16"/>
-    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="N3:P3"/>
     <mergeCell ref="V3:X3"/>
     <mergeCell ref="J8:L8"/>
     <mergeCell ref="B9:D9"/>
@@ -16496,11 +16491,16 @@
     <mergeCell ref="R11:T11"/>
     <mergeCell ref="V11:X11"/>
     <mergeCell ref="R3:T3"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="N16:P16"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="V16:X16"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16552,11 +16552,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="2:37" x14ac:dyDescent="0.2">
       <c r="AB2" s="5" t="s">
@@ -16564,36 +16564,36 @@
       </c>
     </row>
     <row r="3" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
       <c r="F3" s="25" t="s">
         <v>81</v>
       </c>
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="N3" s="20" t="s">
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="N3" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="R3" s="20" t="s">
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="R3" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="V3" s="20" t="s">
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="V3" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="W3" s="20"/>
-      <c r="X3" s="20"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="27"/>
       <c r="AB3" s="6" t="s">
         <v>63</v>
       </c>
@@ -17161,11 +17161,11 @@
       </c>
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
-      <c r="J10" s="24" t="s">
+      <c r="J10" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
       <c r="N10" t="s">
         <v>127</v>
       </c>
@@ -17228,7 +17228,7 @@
       </c>
     </row>
     <row r="11" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="23"/>
@@ -17620,11 +17620,11 @@
       </c>
     </row>
     <row r="16" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
       <c r="F16" t="s">
         <v>103</v>
       </c>
@@ -18384,11 +18384,11 @@
       </c>
     </row>
     <row r="25" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
       <c r="F25" s="3"/>
       <c r="K25" s="1">
         <v>20</v>
@@ -19008,11 +19008,11 @@
       </c>
     </row>
     <row r="35" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
       <c r="F35" t="s">
         <v>114</v>
       </c>
@@ -21699,11 +21699,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="N3:P3"/>
     <mergeCell ref="V3:X3"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="J10:L10"/>
@@ -21712,11 +21712,11 @@
     <mergeCell ref="R15:T15"/>
     <mergeCell ref="V15:X15"/>
     <mergeCell ref="R3:T3"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>